<commit_message>
Actualizacion Puntajes y Entregas
</commit_message>
<xml_diff>
--- a/Documentacion/Metrica de contribucion - WEB.xlsx
+++ b/Documentacion/Metrica de contribucion - WEB.xlsx
@@ -17,15 +17,15 @@
     <t>Tarea</t>
   </si>
   <si>
+    <t>Puntos Actuales</t>
+  </si>
+  <si>
     <t>Encargado</t>
   </si>
   <si>
     <t>Dias de Elaboracion</t>
   </si>
   <si>
-    <t>Puntos Actuales</t>
-  </si>
-  <si>
     <t>Entrega en tiempo</t>
   </si>
   <si>
@@ -47,10 +47,10 @@
     <t>Javier Quijano</t>
   </si>
   <si>
+    <t xml:space="preserve">Puntaje total Posible </t>
+  </si>
+  <si>
     <t>Antonio Barrera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puntaje total Posible </t>
   </si>
   <si>
     <t>Braulio Frias</t>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -166,7 +166,6 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -228,10 +227,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -249,7 +248,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -270,7 +269,9 @@
       <c r="C3" s="8">
         <v>2.0</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="1">
+        <v>1.0</v>
+      </c>
       <c r="E3" s="1">
         <v>2.0</v>
       </c>
@@ -280,7 +281,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8">
         <v>2.0</v>
@@ -302,7 +303,9 @@
       <c r="C5" s="8">
         <v>4.0</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="1">
+        <v>1.0</v>
+      </c>
       <c r="E5" s="1">
         <v>4.0</v>
       </c>
@@ -325,43 +328,43 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
     </row>
     <row r="9">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
     </row>
     <row r="10">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
     </row>
     <row r="12">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
     </row>
     <row r="13">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="10"/>
+      <c r="A14" s="9"/>
     </row>
     <row r="15">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
     </row>
     <row r="16">
-      <c r="A16" s="10"/>
+      <c r="A16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="10"/>
+      <c r="A17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
     </row>
     <row r="19">
-      <c r="A19" s="10"/>
+      <c r="A19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="10"/>
+      <c r="A20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -397,12 +400,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -416,11 +419,11 @@
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" s="5">
         <f>(B3)/'Puntaje por Tareas'!J2</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4">
@@ -428,16 +431,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" s="5">
         <f>(B4)/'Puntaje por Tareas'!J2</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>2.0</v>
@@ -464,11 +467,11 @@
         <v>14</v>
       </c>
       <c r="B7" s="2">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C7" s="5">
         <f>(B7)/'Puntaje por Tareas'!J2</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>